<commit_message>
Logartimización de todas las variables y eliminación de categoricas
</commit_message>
<xml_diff>
--- a/Coeficientes_lasso.xlsx
+++ b/Coeficientes_lasso.xlsx
@@ -74,52 +74,52 @@
     <t>(Intercept)</t>
   </si>
   <si>
-    <t>`pH agua:suelo`</t>
-  </si>
-  <si>
-    <t>`Fósforo Bray II`</t>
-  </si>
-  <si>
-    <t>`Azufre Fosfato monocalcico`</t>
-  </si>
-  <si>
-    <t>`Acidez Intercambiable`</t>
-  </si>
-  <si>
-    <t>`Aluminio intercambiable`</t>
-  </si>
-  <si>
-    <t>`Calcio intercambiable`</t>
-  </si>
-  <si>
-    <t>`Magnesio intercambiable`</t>
-  </si>
-  <si>
-    <t>`Potasio intercambiable`</t>
-  </si>
-  <si>
-    <t>`Sodio intercambiable`</t>
-  </si>
-  <si>
-    <t>`capacidad de intercambio cationico`</t>
-  </si>
-  <si>
-    <t>`Conductividad electrica`</t>
-  </si>
-  <si>
-    <t>`Hierro disponible olsen`</t>
-  </si>
-  <si>
-    <t>`Cobre disponible`</t>
-  </si>
-  <si>
-    <t>`Manganeso disponible Olsen`</t>
-  </si>
-  <si>
-    <t>`Zinc disponible Olsen`</t>
-  </si>
-  <si>
-    <t>`Boro disponible`</t>
+    <t>pH.agua.suelo</t>
+  </si>
+  <si>
+    <t>Fósforo.Bray.II</t>
+  </si>
+  <si>
+    <t>Azufre.Fosfato.monocalcico</t>
+  </si>
+  <si>
+    <t>Acidez.Intercambiable</t>
+  </si>
+  <si>
+    <t>Aluminio.intercambiable</t>
+  </si>
+  <si>
+    <t>Calcio.intercambiable</t>
+  </si>
+  <si>
+    <t>Magnesio.intercambiable</t>
+  </si>
+  <si>
+    <t>Potasio.intercambiable</t>
+  </si>
+  <si>
+    <t>Sodio.intercambiable</t>
+  </si>
+  <si>
+    <t>capacidad.de.intercambio.cationico</t>
+  </si>
+  <si>
+    <t>Conductividad.electrica</t>
+  </si>
+  <si>
+    <t>Hierro.disponible.olsen</t>
+  </si>
+  <si>
+    <t>Cobre.disponible</t>
+  </si>
+  <si>
+    <t>Manganeso.disponible.Olsen</t>
+  </si>
+  <si>
+    <t>Zinc.disponible.Olsen</t>
+  </si>
+  <si>
+    <t>Boro.disponible</t>
   </si>
 </sst>
 </file>
@@ -187,7 +187,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="n">
-        <v>1.9779788155239642</v>
+        <v>2.1454175777854183</v>
       </c>
     </row>
     <row r="3">
@@ -198,7 +198,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>0.20236020274320055</v>
+        <v>0.44762115175654044</v>
       </c>
     </row>
     <row r="4">
@@ -220,7 +220,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0</v>
+        <v>0.012413611575142378</v>
       </c>
     </row>
     <row r="6">
@@ -231,7 +231,7 @@
         <v>23</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>0.07902442609122665</v>
       </c>
     </row>
     <row r="7">
@@ -242,7 +242,7 @@
         <v>24</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>0.06512373023491637</v>
       </c>
     </row>
     <row r="8">
@@ -264,7 +264,7 @@
         <v>26</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.2548898485179404</v>
+        <v>-0.1650672261683916</v>
       </c>
     </row>
     <row r="10">
@@ -275,7 +275,7 @@
         <v>27</v>
       </c>
       <c r="C10" t="n">
-        <v>0.16874845534438623</v>
+        <v>0.12292377958328944</v>
       </c>
     </row>
     <row r="11">
@@ -286,7 +286,7 @@
         <v>28</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.06619066689844139</v>
+        <v>-0.11406705779358295</v>
       </c>
     </row>
     <row r="12">
@@ -297,7 +297,7 @@
         <v>29</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.051266530287851504</v>
+        <v>-0.15889824917456358</v>
       </c>
     </row>
     <row r="13">
@@ -308,7 +308,7 @@
         <v>30</v>
       </c>
       <c r="C13" t="n">
-        <v>0.10926731767595263</v>
+        <v>0.18270469928597377</v>
       </c>
     </row>
     <row r="14">
@@ -319,7 +319,7 @@
         <v>31</v>
       </c>
       <c r="C14" t="n">
-        <v>0.06717202602064873</v>
+        <v>0.07593913294443458</v>
       </c>
     </row>
     <row r="15">
@@ -341,7 +341,7 @@
         <v>33</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.04324667952533741</v>
+        <v>-0.07845058366124621</v>
       </c>
     </row>
     <row r="17">
@@ -352,7 +352,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="n">
-        <v>0.07983297117258005</v>
+        <v>0.10460414134404898</v>
       </c>
     </row>
     <row r="18">
@@ -363,7 +363,7 @@
         <v>35</v>
       </c>
       <c r="C18" t="n">
-        <v>0.004718366834642036</v>
+        <v>-0.002902555094178036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Opcion de Winzorizacion y actualización modelo Ridge
</commit_message>
<xml_diff>
--- a/Coeficientes_lasso.xlsx
+++ b/Coeficientes_lasso.xlsx
@@ -187,7 +187,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="n">
-        <v>2.1454175777854183</v>
+        <v>2.111455329893493</v>
       </c>
     </row>
     <row r="3">
@@ -198,7 +198,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>0.44762115175654044</v>
+        <v>0.3920205665085499</v>
       </c>
     </row>
     <row r="4">
@@ -209,7 +209,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0</v>
+        <v>-0.014504764799976004</v>
       </c>
     </row>
     <row r="5">
@@ -220,7 +220,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="n">
-        <v>0.012413611575142378</v>
+        <v>0.034827692605432635</v>
       </c>
     </row>
     <row r="6">
@@ -231,7 +231,7 @@
         <v>23</v>
       </c>
       <c r="C6" t="n">
-        <v>0.07902442609122665</v>
+        <v>0.06803680322205402</v>
       </c>
     </row>
     <row r="7">
@@ -242,7 +242,7 @@
         <v>24</v>
       </c>
       <c r="C7" t="n">
-        <v>0.06512373023491637</v>
+        <v>0.06792839823741074</v>
       </c>
     </row>
     <row r="8">
@@ -253,7 +253,7 @@
         <v>25</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0</v>
+        <v>0.022551890854185363</v>
       </c>
     </row>
     <row r="9">
@@ -264,7 +264,7 @@
         <v>26</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.1650672261683916</v>
+        <v>-0.15717406572951634</v>
       </c>
     </row>
     <row r="10">
@@ -275,7 +275,7 @@
         <v>27</v>
       </c>
       <c r="C10" t="n">
-        <v>0.12292377958328944</v>
+        <v>0.13454098486900007</v>
       </c>
     </row>
     <row r="11">
@@ -286,7 +286,7 @@
         <v>28</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.11406705779358295</v>
+        <v>-0.11289894807040429</v>
       </c>
     </row>
     <row r="12">
@@ -297,7 +297,7 @@
         <v>29</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.15889824917456358</v>
+        <v>-0.16436059978959433</v>
       </c>
     </row>
     <row r="13">
@@ -308,7 +308,7 @@
         <v>30</v>
       </c>
       <c r="C13" t="n">
-        <v>0.18270469928597377</v>
+        <v>0.17943849699314326</v>
       </c>
     </row>
     <row r="14">
@@ -319,7 +319,7 @@
         <v>31</v>
       </c>
       <c r="C14" t="n">
-        <v>0.07593913294443458</v>
+        <v>0.07835671027811729</v>
       </c>
     </row>
     <row r="15">
@@ -330,7 +330,7 @@
         <v>32</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0</v>
+        <v>-0.007718421908448897</v>
       </c>
     </row>
     <row r="16">
@@ -341,7 +341,7 @@
         <v>33</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.07845058366124621</v>
+        <v>-0.08035286371511285</v>
       </c>
     </row>
     <row r="17">
@@ -352,7 +352,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="n">
-        <v>0.10460414134404898</v>
+        <v>0.1051118163046719</v>
       </c>
     </row>
     <row r="18">
@@ -363,7 +363,7 @@
         <v>35</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.002902555094178036</v>
+        <v>-0.010810943718758377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>